<commit_message>
yeah have some updates my g
</commit_message>
<xml_diff>
--- a/JLC_BOM.xlsx
+++ b/JLC_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunostjohn/Documents/Button MIDI Controller/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{565EEE31-2744-1F46-B810-3CDE823C92FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84F62836-CA35-CE4D-AE82-7C9668EEF4A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="920" windowWidth="34240" windowHeight="20200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -61,21 +61,12 @@
     <t>C4,C5,C6,C16</t>
   </si>
   <si>
-    <t>C7-C15</t>
-  </si>
-  <si>
     <t>10uF</t>
   </si>
   <si>
     <t>C17</t>
   </si>
   <si>
-    <t>D1-D64</t>
-  </si>
-  <si>
-    <t>D65-D192</t>
-  </si>
-  <si>
     <t>WS2812B</t>
   </si>
   <si>
@@ -85,9 +76,6 @@
     <t>PLCC4 2mm x 2mm</t>
   </si>
   <si>
-    <t>D193-D199</t>
-  </si>
-  <si>
     <t>500mA</t>
   </si>
   <si>
@@ -218,6 +206,18 @@
   </si>
   <si>
     <t>C9002</t>
+  </si>
+  <si>
+    <t>C7-15</t>
+  </si>
+  <si>
+    <t>D65-192</t>
+  </si>
+  <si>
+    <t>D193-199</t>
+  </si>
+  <si>
+    <t>D1-64</t>
   </si>
 </sst>
 </file>
@@ -235,7 +235,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -316,7 +316,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -665,7 +665,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:D20"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="20" customHeight="1"/>
@@ -687,7 +687,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="1" customFormat="1" ht="20" customHeight="1">
@@ -701,7 +701,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="1" customFormat="1" ht="20" customHeight="1">
@@ -715,7 +715,7 @@
         <v>7</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="1" customFormat="1" ht="20" customHeight="1">
@@ -729,7 +729,7 @@
         <v>7</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="1" customFormat="1" ht="20" customHeight="1">
@@ -742,210 +742,210 @@
       <c r="C5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>50</v>
+      <c r="D5" s="7" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="1" customFormat="1" ht="20" customHeight="1">
       <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>13</v>
+      <c r="B6" s="7" t="s">
+        <v>62</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="1" customFormat="1" ht="20" customHeight="1">
       <c r="A7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="1" customFormat="1" ht="20" customHeight="1">
       <c r="A8" s="4"/>
-      <c r="B8" s="3" t="s">
-        <v>16</v>
+      <c r="B8" s="7" t="s">
+        <v>65</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="20" customHeight="1">
       <c r="A9" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B9" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="D9" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="20" customHeight="1">
       <c r="A10" s="4"/>
       <c r="B10" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>53</v>
+        <v>64</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="20" customHeight="1">
       <c r="A11" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>24</v>
+        <v>18</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="20" customHeight="1">
       <c r="A12" s="4"/>
-      <c r="B12" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>26</v>
+      <c r="B12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="20" customHeight="1">
       <c r="A13" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>58</v>
+        <v>23</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="20" customHeight="1">
       <c r="A14" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>59</v>
+        <v>26</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="20" customHeight="1">
       <c r="A15" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>29</v>
       </c>
+      <c r="C15" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="D15" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="20" customHeight="1">
       <c r="A16" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>29</v>
+        <v>30</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="20" customHeight="1">
       <c r="A17" s="4"/>
-      <c r="B17" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>37</v>
+      <c r="B17" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="20" customHeight="1">
       <c r="A18" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B18" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="7" t="s">
-        <v>39</v>
+      <c r="B18" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="20" customHeight="1">
       <c r="A19" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="20" customHeight="1">
       <c r="A20" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>45</v>
+        <v>42</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>